<commit_message>
Sun May 31 23:28:16 MDT 2015
</commit_message>
<xml_diff>
--- a/ICBP_Drug_Classes.xlsx
+++ b/ICBP_Drug_Classes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="164">
   <si>
     <t>X17.AAG</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>Class 1</t>
+  </si>
+  <si>
+    <t>VEGFR, Raf</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,12 +582,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,7 +614,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1567,7 +1564,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="78" spans="1:2">

</xml_diff>

<commit_message>
Thu Aug 13 02:39:15 CDT 2015
</commit_message>
<xml_diff>
--- a/ICBP_Drug_Classes.xlsx
+++ b/ICBP_Drug_Classes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="8680" windowHeight="18420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="165">
   <si>
     <t>X17.AAG</t>
   </si>
@@ -542,6 +542,9 @@
   </si>
   <si>
     <t>VEGFR, Raf</t>
+  </si>
+  <si>
+    <t>CDK4 inhibitor</t>
   </si>
 </sst>
 </file>
@@ -950,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1177,6 +1180,9 @@
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B28" s="5" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">

</xml_diff>